<commit_message>
Modified the Transfer Curves
</commit_message>
<xml_diff>
--- a/UnitTests/DriveForwards/TransferCurveData.xlsx
+++ b/UnitTests/DriveForwards/TransferCurveData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="TransferCurveData" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <t>Pulse Width (us)</t>
   </si>
   <si>
-    <t>Right Servo Rotational Velocity (RPM CW(-) CCW(+))</t>
+    <t>Right Servo Rotational Velocity (RPM CW(+) CCW(-))</t>
   </si>
   <si>
     <t>Left Servo Rotatinal Velocity (RPM CW(-) CCW(+))</t>
@@ -592,12 +592,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -605,7 +612,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Transfer Curve Data</a:t>
+              <a:t>Transfer Curve for BoeBot Servo Calibration</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -624,12 +631,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -649,50 +663,80 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Right Servo</c:v>
+            <c:strRef>
+              <c:f>TransferCurveData!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Right Servo Rotational Velocity (RPM CW(+) CCW(-))</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
             </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
               </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>TransferCurveData!$A$2:$A$18</c:f>
+              <c:f>TransferCurveData!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1300</c:v>
                 </c:pt>
@@ -736,12 +780,18 @@
                   <c:v>1625</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>1635</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1638</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>1675</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>1700</c:v>
                 </c:pt>
               </c:numCache>
@@ -749,60 +799,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TransferCurveData!$B$2:$B$18</c:f>
+              <c:f>TransferCurveData!$B$2:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>-50</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-50</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-49.6</c:v>
+                  <c:v>49.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-49</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-48</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-44</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-32.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-16</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31</c:v>
+                  <c:v>-31</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42.5</c:v>
+                  <c:v>-42.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>47.5</c:v>
+                  <c:v>-47.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49.5</c:v>
+                  <c:v>-49.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50</c:v>
+                  <c:v>-49.8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>-50</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>50</c:v>
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -813,50 +869,80 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Left Servo</c:v>
+            <c:strRef>
+              <c:f>TransferCurveData!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left Servo Rotatinal Velocity (RPM CW(-) CCW(+))</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
             </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
               </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>TransferCurveData!$A$2:$A$18</c:f>
+              <c:f>TransferCurveData!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1300</c:v>
                 </c:pt>
@@ -900,12 +986,18 @@
                   <c:v>1625</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>1635</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1638</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>1675</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>1700</c:v>
                 </c:pt>
               </c:numCache>
@@ -913,10 +1005,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TransferCurveData!$C$2:$C$18</c:f>
+              <c:f>TransferCurveData!$C$2:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>-50</c:v>
                 </c:pt>
@@ -957,15 +1049,21 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49</c:v>
+                  <c:v>47.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>47.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>49.4</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>49.8</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>49.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -981,11 +1079,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="373998808"/>
-        <c:axId val="373999984"/>
+        <c:axId val="307464664"/>
+        <c:axId val="307463096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="373998808"/>
+        <c:axId val="307464664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1200"/>
@@ -996,10 +1094,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1014,7 +1111,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -1046,7 +1143,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
@@ -1067,8 +1164,12 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1091,12 +1192,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373999984"/>
+        <c:crossAx val="307463096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="373999984"/>
+        <c:axId val="307463096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,10 +1207,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1124,7 +1224,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -1156,7 +1256,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
@@ -1183,7 +1283,6 @@
                 <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1206,7 +1305,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373998808"/>
+        <c:crossAx val="307464664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1219,7 +1318,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1254,20 +1353,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1330,7 +1437,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1340,7 +1447,7 @@
         <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1351,6 +1458,15 @@
         <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea>
@@ -1361,23 +1477,28 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1395,17 +1516,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1414,131 +1532,72 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1561,9 +1620,9 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1575,22 +1634,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1599,16 +1658,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1617,13 +1677,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1635,7 +1695,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -1648,10 +1708,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1666,15 +1725,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1683,73 +1740,83 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1757,13 +1824,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1776,10 +1844,18 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1788,15 +1864,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="25400" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1816,21 +1891,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1850,18 +1923,16 @@
             <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -1871,20 +1942,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>201779</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38350</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>150394</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>25065</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2165,10 +2236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="92" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,7 +2260,7 @@
         <v>1300</v>
       </c>
       <c r="B2">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>-50</v>
@@ -2200,7 +2271,7 @@
         <v>1325</v>
       </c>
       <c r="B3">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>-49.9</v>
@@ -2211,7 +2282,7 @@
         <v>1350</v>
       </c>
       <c r="B4">
-        <v>-49.6</v>
+        <v>49.6</v>
       </c>
       <c r="C4">
         <v>-50</v>
@@ -2222,7 +2293,7 @@
         <v>1375</v>
       </c>
       <c r="B5">
-        <v>-49</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>-49</v>
@@ -2233,7 +2304,7 @@
         <v>1400</v>
       </c>
       <c r="B6">
-        <v>-48</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>-47.5</v>
@@ -2244,7 +2315,7 @@
         <v>1425</v>
       </c>
       <c r="B7">
-        <v>-44</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>-44</v>
@@ -2255,7 +2326,7 @@
         <v>1450</v>
       </c>
       <c r="B8">
-        <v>-32.5</v>
+        <v>32.5</v>
       </c>
       <c r="C8">
         <v>-32.5</v>
@@ -2266,7 +2337,7 @@
         <v>1475</v>
       </c>
       <c r="B9">
-        <v>-16</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>-16.600000000000001</v>
@@ -2288,7 +2359,7 @@
         <v>1525</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>-14</v>
       </c>
       <c r="C11">
         <v>13.9</v>
@@ -2299,7 +2370,7 @@
         <v>1550</v>
       </c>
       <c r="B12">
-        <v>31</v>
+        <v>-31</v>
       </c>
       <c r="C12">
         <v>30.5</v>
@@ -2310,7 +2381,7 @@
         <v>1575</v>
       </c>
       <c r="B13">
-        <v>42.5</v>
+        <v>-42.5</v>
       </c>
       <c r="C13">
         <v>41</v>
@@ -2321,7 +2392,7 @@
         <v>1600</v>
       </c>
       <c r="B14">
-        <v>47.5</v>
+        <v>-47.5</v>
       </c>
       <c r="C14">
         <v>46</v>
@@ -2332,42 +2403,64 @@
         <v>1625</v>
       </c>
       <c r="B15">
-        <v>49.5</v>
+        <v>-49.5</v>
       </c>
       <c r="C15">
-        <v>49</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1650</v>
+        <v>1635</v>
       </c>
       <c r="B16">
-        <v>50</v>
+        <v>-49.8</v>
       </c>
       <c r="C16">
-        <v>49.4</v>
+        <v>47.9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1675</v>
+        <v>1638</v>
       </c>
       <c r="B17">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="C17">
-        <v>49.8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>1650</v>
+      </c>
+      <c r="B18">
+        <v>-50</v>
+      </c>
+      <c r="C18">
+        <v>49.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1675</v>
+      </c>
+      <c r="B19">
+        <v>-50</v>
+      </c>
+      <c r="C19">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>1700</v>
       </c>
-      <c r="B18">
-        <v>50</v>
-      </c>
-      <c r="C18">
+      <c r="B20">
+        <v>-50</v>
+      </c>
+      <c r="C20">
         <v>49.5</v>
       </c>
     </row>

</xml_diff>